<commit_message>
Update 2023-567-Exam 2 - Control Chart Question Data-1.xlsx
</commit_message>
<xml_diff>
--- a/2023-567-Exam 2 - Control Chart Question Data-1.xlsx
+++ b/2023-567-Exam 2 - Control Chart Question Data-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D-Developer\UIUC-BADM567-Process-Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3007F44-03EE-4334-9BBB-BF432260AEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4F2368-EBAD-49A1-BBA9-1DE5FEF6682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1140" windowWidth="20280" windowHeight="14640" xr2:uid="{6D7D1BB6-8DFD-4B65-B980-BA31D0E768DF}"/>
+    <workbookView xWindow="20320" yWindow="2990" windowWidth="15330" windowHeight="14640" xr2:uid="{6D7D1BB6-8DFD-4B65-B980-BA31D0E768DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -110,7 +110,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -314,6 +314,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -328,12 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,36 +651,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71742AE8-4A2E-40A5-A45B-B051576DFF91}">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="10" max="13" width="12.4140625" customWidth="1"/>
+    <col min="10" max="13" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="14.5" thickBot="1"/>
+    <row r="1" spans="2:13" ht="15" thickBot="1"/>
     <row r="2" spans="2:13" ht="62.5" customHeight="1" thickBot="1">
       <c r="B2" s="1"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -706,10 +706,10 @@
       <c r="H3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:13" ht="16" thickBot="1">
       <c r="B4" s="7">
@@ -846,16 +846,16 @@
         <f t="shared" si="1"/>
         <v>0.59999999999999964</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="12">
         <v>5</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="13">
         <v>0.57699999999999996</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="13">
         <v>0</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="13">
         <v>2.1139999999999999</v>
       </c>
     </row>

</xml_diff>